<commit_message>
Updated new standards, and added 27P as a new site for review
</commit_message>
<xml_diff>
--- a/files/compliance_standards.xlsx
+++ b/files/compliance_standards.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olato\PycharmProjects\site_qa_review\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0030B6F5-D4FB-4D29-BFE3-51930FA4A311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C159F4F-4D29-480A-BC7D-7FA58D53FD08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1230" yWindow="1260" windowWidth="22605" windowHeight="14205" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TOBOLA Standards" sheetId="3" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1420" uniqueCount="533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1429" uniqueCount="540">
   <si>
     <t>SECTION</t>
   </si>
@@ -1428,9 +1428,6 @@
   </si>
   <si>
     <t>Support Needs Document</t>
-  </si>
-  <si>
-    <t>For each individual, an updated Support Needs Document should be accessible in THERAP and is valid for 1 year after approval.</t>
   </si>
   <si>
     <t>01 OPENING A HOME</t>
@@ -1648,6 +1645,30 @@
   </si>
   <si>
     <t>Each provider shall cooperate fully with the Medicaid Fraud Control Unit and the state protection and advocacy agency, as defined in 16 Del.C. §11l2(7), in fulfilling functions authorized by 16 http://del.c.ch/. 11.</t>
+  </si>
+  <si>
+    <t>Sade Ojo</t>
+  </si>
+  <si>
+    <t>For each individual, an updated Support Needs Document should be accessible in THERAP and is valid for 1 year after approval or last update</t>
+  </si>
+  <si>
+    <t>All sites will hold monthly house meetings with the service recipients at the program, to identify their wants, needs, and plans for the next month. As well as the coordination of any outings, visits, appointments, and so on. The meeting agenda, sign-in, and minutes must be uploaded to Notion for documentation tracking</t>
+  </si>
+  <si>
+    <t>House Meetings</t>
+  </si>
+  <si>
+    <t>Staff Meetings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All sites will hold monthly staff meetings with all of the full time, part time, and prn staff assigned to the site. These meetings are used to ensure effective communication between all levels within TOBOLA. The meeting agenda, sign-in, and minutes must be uploaded to Notion for documentation tracking. </t>
+  </si>
+  <si>
+    <t>EMAR Report</t>
+  </si>
+  <si>
+    <t>At the end of each month, each service recipient that recieves medications will have a report printed out of their EMAR for the month. This EMAR printout must be placed into the individuals Physical MAR binder, along with any scripts, D/C's, or any other relevant information to that service recipient for that month.</t>
   </si>
 </sst>
 </file>
@@ -2180,7 +2201,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2209,6 +2230,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2262,13 +2284,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2282,6 +2301,9 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2303,8 +2325,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0A445865-36BF-446D-BBBC-83B2A2E02B82}" name="Table14" displayName="Table14" ref="A1:D22" totalsRowShown="0">
-  <autoFilter ref="A1:D22" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0A445865-36BF-446D-BBBC-83B2A2E02B82}" name="Table14" displayName="Table14" ref="A1:D25" totalsRowShown="0">
+  <autoFilter ref="A1:D25" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B22">
     <sortCondition ref="A2:A22"/>
   </sortState>
@@ -2312,23 +2334,23 @@
     <tableColumn id="1" xr3:uid="{3146BF90-4351-420E-AD7B-71EC07B07460}" name="SECTION"/>
     <tableColumn id="2" xr3:uid="{A829C56E-094A-4A1F-90B4-88E1AB092D31}" name="STANDARD" dataDxfId="10"/>
     <tableColumn id="8" xr3:uid="{749BDD54-2E9E-4CA0-B48B-B509B08CBA51}" name="DESCRIPTION" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{789CE3AA-C749-4983-AEC6-DC6BDDCB7B0B}" name="Default" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{789CE3AA-C749-4983-AEC6-DC6BDDCB7B0B}" name="Default" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F56633E1-3A94-4ABD-834C-8F3277A204A4}" name="Table13" displayName="Table13" ref="A1:D255" totalsRowShown="0" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F56633E1-3A94-4ABD-834C-8F3277A204A4}" name="Table13" displayName="Table13" ref="A1:D255" totalsRowShown="0" dataDxfId="7">
   <autoFilter ref="A1:D255" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B255">
     <sortCondition ref="A2:A255"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{B5F57C1F-71D7-4E66-B159-26F7D14FC333}" name="SECTION" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{8B79EBC4-0FA0-4ED6-83BC-6D50A229E88F}" name="STANDARD" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{D1A93CC0-0AD4-4552-B397-F625E00D7481}" name="DESCRIPTION" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{E2A926BA-8133-41A3-B146-0FEF5CEBCC92}" name="Default" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{B5F57C1F-71D7-4E66-B159-26F7D14FC333}" name="SECTION" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{8B79EBC4-0FA0-4ED6-83BC-6D50A229E88F}" name="STANDARD" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{D1A93CC0-0AD4-4552-B397-F625E00D7481}" name="DESCRIPTION" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{E2A926BA-8133-41A3-B146-0FEF5CEBCC92}" name="Default" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2343,9 +2365,9 @@
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="SECTION"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="STANDARD" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="DESCRIPTION" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{2B589D88-A3B1-4636-AA64-F6C8E3997C17}" name="Default" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="STANDARD" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="DESCRIPTION" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{2B589D88-A3B1-4636-AA64-F6C8E3997C17}" name="Default" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2651,10 +2673,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2670,13 +2692,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -2708,7 +2730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -2716,7 +2738,7 @@
         <v>461</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>462</v>
+        <v>533</v>
       </c>
       <c r="D4" s="1" t="b">
         <v>0</v>
@@ -2772,7 +2794,7 @@
         <v>331</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D8" s="1" t="b">
         <v>0</v>
@@ -2971,6 +2993,48 @@
         <v>304</v>
       </c>
       <c r="D22" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>535</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="D23" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>536</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="D24" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>538</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="D25" s="1" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2990,8 +3054,8 @@
   </sheetPr>
   <dimension ref="A1:D255"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14:D255"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3008,18 +3072,18 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>218</v>
@@ -3033,7 +3097,7 @@
     </row>
     <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>332</v>
@@ -3047,7 +3111,7 @@
     </row>
     <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>42</v>
@@ -3061,7 +3125,7 @@
     </row>
     <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>84</v>
@@ -3075,7 +3139,7 @@
     </row>
     <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>120</v>
@@ -3089,7 +3153,7 @@
     </row>
     <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>82</v>
@@ -3103,7 +3167,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>179</v>
@@ -3117,7 +3181,7 @@
     </row>
     <row r="9" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B9" s="13" t="s">
         <v>353</v>
@@ -3131,7 +3195,7 @@
     </row>
     <row r="10" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B10" s="13" t="s">
         <v>118</v>
@@ -3145,7 +3209,7 @@
     </row>
     <row r="11" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>174</v>
@@ -3159,7 +3223,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>204</v>
@@ -3173,7 +3237,7 @@
     </row>
     <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B13" s="13" t="s">
         <v>220</v>
@@ -3187,7 +3251,7 @@
     </row>
     <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B14" s="13" t="s">
         <v>359</v>
@@ -3201,7 +3265,7 @@
     </row>
     <row r="15" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B15" s="13" t="s">
         <v>382</v>
@@ -3215,7 +3279,7 @@
     </row>
     <row r="16" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B16" s="13" t="s">
         <v>440</v>
@@ -3229,7 +3293,7 @@
     </row>
     <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B17" s="13" t="s">
         <v>273</v>
@@ -3243,7 +3307,7 @@
     </row>
     <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B18" s="15" t="s">
         <v>255</v>
@@ -3257,7 +3321,7 @@
     </row>
     <row r="19" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B19" s="13" t="s">
         <v>394</v>
@@ -3271,7 +3335,7 @@
     </row>
     <row r="20" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B20" s="13" t="s">
         <v>385</v>
@@ -3285,7 +3349,7 @@
     </row>
     <row r="21" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B21" s="13" t="s">
         <v>198</v>
@@ -3299,7 +3363,7 @@
     </row>
     <row r="22" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B22" s="13" t="s">
         <v>275</v>
@@ -3313,7 +3377,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B23" s="15" t="s">
         <v>53</v>
@@ -3327,7 +3391,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B24" s="15" t="s">
         <v>271</v>
@@ -3341,7 +3405,7 @@
     </row>
     <row r="25" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B25" s="15" t="s">
         <v>186</v>
@@ -3355,7 +3419,7 @@
     </row>
     <row r="26" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B26" s="15" t="s">
         <v>194</v>
@@ -3369,13 +3433,13 @@
     </row>
     <row r="27" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B27" s="15" t="s">
         <v>245</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D27" s="14" t="b">
         <v>1</v>
@@ -3383,7 +3447,7 @@
     </row>
     <row r="28" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B28" s="15" t="s">
         <v>369</v>
@@ -3397,7 +3461,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B29" s="15" t="s">
         <v>321</v>
@@ -3411,7 +3475,7 @@
     </row>
     <row r="30" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A30" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B30" s="15" t="s">
         <v>338</v>
@@ -3425,7 +3489,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B31" s="13" t="s">
         <v>420</v>
@@ -3439,7 +3503,7 @@
     </row>
     <row r="32" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B32" s="15" t="s">
         <v>57</v>
@@ -3453,7 +3517,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B33" s="15" t="s">
         <v>70</v>
@@ -3467,7 +3531,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B34" s="15" t="s">
         <v>37</v>
@@ -3481,7 +3545,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B35" s="13" t="s">
         <v>47</v>
@@ -3495,7 +3559,7 @@
     </row>
     <row r="36" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B36" s="15" t="s">
         <v>259</v>
@@ -3509,7 +3573,7 @@
     </row>
     <row r="37" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B37" s="15" t="s">
         <v>161</v>
@@ -3523,7 +3587,7 @@
     </row>
     <row r="38" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B38" s="13" t="s">
         <v>78</v>
@@ -3537,7 +3601,7 @@
     </row>
     <row r="39" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B39" s="15" t="s">
         <v>2</v>
@@ -3551,7 +3615,7 @@
     </row>
     <row r="40" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B40" s="15" t="s">
         <v>336</v>
@@ -3565,7 +3629,7 @@
     </row>
     <row r="41" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B41" s="15" t="s">
         <v>267</v>
@@ -3579,7 +3643,7 @@
     </row>
     <row r="42" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B42" s="15" t="s">
         <v>68</v>
@@ -3593,7 +3657,7 @@
     </row>
     <row r="43" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A43" s="12" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B43" s="13" t="s">
         <v>231</v>
@@ -3607,13 +3671,13 @@
     </row>
     <row r="44" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A44" s="12" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B44" s="13" t="s">
         <v>144</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D44" s="14" t="b">
         <v>1</v>
@@ -3621,7 +3685,7 @@
     </row>
     <row r="45" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A45" s="12" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B45" s="13" t="s">
         <v>212</v>
@@ -3635,7 +3699,7 @@
     </row>
     <row r="46" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" s="12" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B46" s="13" t="s">
         <v>342</v>
@@ -3649,13 +3713,13 @@
     </row>
     <row r="47" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="12" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B47" s="13" t="s">
         <v>261</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D47" s="14" t="b">
         <v>1</v>
@@ -3663,7 +3727,7 @@
     </row>
     <row r="48" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="12" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B48" s="13" t="s">
         <v>305</v>
@@ -3677,13 +3741,13 @@
     </row>
     <row r="49" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A49" s="12" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B49" s="13" t="s">
         <v>17</v>
       </c>
       <c r="C49" s="14" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D49" s="14" t="b">
         <v>1</v>
@@ -3691,7 +3755,7 @@
     </row>
     <row r="50" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="12" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B50" s="15" t="s">
         <v>448</v>
@@ -3705,7 +3769,7 @@
     </row>
     <row r="51" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A51" s="12" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B51" s="13" t="s">
         <v>313</v>
@@ -3719,7 +3783,7 @@
     </row>
     <row r="52" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A52" s="12" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B52" s="13" t="s">
         <v>265</v>
@@ -3733,7 +3797,7 @@
     </row>
     <row r="53" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="12" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B53" s="15" t="s">
         <v>400</v>
@@ -3747,7 +3811,7 @@
     </row>
     <row r="54" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="12" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B54" s="15" t="s">
         <v>288</v>
@@ -3761,7 +3825,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="12" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B55" s="15" t="s">
         <v>422</v>
@@ -3775,7 +3839,7 @@
     </row>
     <row r="56" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A56" s="12" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B56" s="15" t="s">
         <v>112</v>
@@ -3789,7 +3853,7 @@
     </row>
     <row r="57" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A57" s="12" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B57" s="13" t="s">
         <v>263</v>
@@ -3803,7 +3867,7 @@
     </row>
     <row r="58" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A58" s="12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B58" s="13" t="s">
         <v>22</v>
@@ -3817,7 +3881,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B59" s="15" t="s">
         <v>238</v>
@@ -3831,7 +3895,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B60" s="15" t="s">
         <v>455</v>
@@ -3845,7 +3909,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B61" s="15" t="s">
         <v>349</v>
@@ -3859,7 +3923,7 @@
     </row>
     <row r="62" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A62" s="12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B62" s="15" t="s">
         <v>437</v>
@@ -3873,7 +3937,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B63" s="15" t="s">
         <v>125</v>
@@ -3887,7 +3951,7 @@
     </row>
     <row r="64" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A64" s="12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B64" s="13" t="s">
         <v>114</v>
@@ -3901,7 +3965,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B65" s="15" t="s">
         <v>157</v>
@@ -3915,7 +3979,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B66" s="15" t="s">
         <v>309</v>
@@ -3929,7 +3993,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B67" s="15" t="s">
         <v>210</v>
@@ -3943,7 +4007,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B68" s="15" t="s">
         <v>99</v>
@@ -3957,7 +4021,7 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B69" s="15" t="s">
         <v>55</v>
@@ -3971,7 +4035,7 @@
     </row>
     <row r="70" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A70" s="12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B70" s="15" t="s">
         <v>328</v>
@@ -3985,7 +4049,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B71" s="15" t="s">
         <v>250</v>
@@ -3999,7 +4063,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B72" s="15" t="s">
         <v>281</v>
@@ -4013,7 +4077,7 @@
     </row>
     <row r="73" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A73" s="12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B73" s="13" t="s">
         <v>363</v>
@@ -4027,7 +4091,7 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B74" s="13" t="s">
         <v>442</v>
@@ -4041,7 +4105,7 @@
     </row>
     <row r="75" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A75" s="12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B75" s="15" t="s">
         <v>451</v>
@@ -4055,7 +4119,7 @@
     </row>
     <row r="76" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A76" s="12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B76" s="15" t="s">
         <v>106</v>
@@ -4069,7 +4133,7 @@
     </row>
     <row r="77" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A77" s="12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B77" s="15" t="s">
         <v>296</v>
@@ -4083,7 +4147,7 @@
     </row>
     <row r="78" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A78" s="12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B78" s="15" t="s">
         <v>404</v>
@@ -4097,7 +4161,7 @@
     </row>
     <row r="79" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A79" s="12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B79" s="15" t="s">
         <v>66</v>
@@ -4111,7 +4175,7 @@
     </row>
     <row r="80" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A80" s="12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B80" s="13" t="s">
         <v>298</v>
@@ -4125,7 +4189,7 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B81" s="13" t="s">
         <v>409</v>
@@ -4139,7 +4203,7 @@
     </row>
     <row r="82" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A82" s="12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B82" s="13" t="s">
         <v>177</v>
@@ -4153,7 +4217,7 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B83" s="15" t="s">
         <v>122</v>
@@ -4167,7 +4231,7 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B84" s="15" t="s">
         <v>87</v>
@@ -4181,7 +4245,7 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B85" s="15" t="s">
         <v>51</v>
@@ -4195,7 +4259,7 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B86" s="15" t="s">
         <v>240</v>
@@ -4209,7 +4273,7 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B87" s="15" t="s">
         <v>453</v>
@@ -4223,7 +4287,7 @@
     </row>
     <row r="88" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A88" s="12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B88" s="15" t="s">
         <v>184</v>
@@ -4237,7 +4301,7 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="12" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B89" s="13" t="s">
         <v>326</v>
@@ -4251,7 +4315,7 @@
     </row>
     <row r="90" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A90" s="12" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B90" s="13" t="s">
         <v>407</v>
@@ -4265,7 +4329,7 @@
     </row>
     <row r="91" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A91" s="12" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B91" s="13" t="s">
         <v>458</v>
@@ -4279,7 +4343,7 @@
     </row>
     <row r="92" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A92" s="12" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B92" s="13" t="s">
         <v>315</v>
@@ -4293,7 +4357,7 @@
     </row>
     <row r="93" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A93" s="12" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B93" s="13" t="s">
         <v>166</v>
@@ -4307,7 +4371,7 @@
     </row>
     <row r="94" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A94" s="12" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B94" s="13" t="s">
         <v>76</v>
@@ -4321,7 +4385,7 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="12" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B95" s="13" t="s">
         <v>323</v>
@@ -4335,13 +4399,13 @@
     </row>
     <row r="96" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A96" s="12" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B96" s="15" t="s">
         <v>146</v>
       </c>
       <c r="C96" s="14" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D96" s="14" t="b">
         <v>0</v>
@@ -4349,7 +4413,7 @@
     </row>
     <row r="97" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A97" s="12" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B97" s="15" t="s">
         <v>269</v>
@@ -4363,7 +4427,7 @@
     </row>
     <row r="98" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A98" s="12" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B98" s="15" t="s">
         <v>413</v>
@@ -4377,7 +4441,7 @@
     </row>
     <row r="99" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A99" s="12" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B99" s="13" t="s">
         <v>444</v>
@@ -4391,7 +4455,7 @@
     </row>
     <row r="100" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A100" s="12" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B100" s="13" t="s">
         <v>429</v>
@@ -4405,7 +4469,7 @@
     </row>
     <row r="101" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A101" s="12" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B101" s="13" t="s">
         <v>357</v>
@@ -4419,7 +4483,7 @@
     </row>
     <row r="102" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A102" s="12" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B102" s="13" t="s">
         <v>340</v>
@@ -4433,7 +4497,7 @@
     </row>
     <row r="103" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A103" s="12" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B103" s="13" t="s">
         <v>376</v>
@@ -4447,7 +4511,7 @@
     </row>
     <row r="104" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A104" s="12" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B104" s="13" t="s">
         <v>62</v>
@@ -4461,7 +4525,7 @@
     </row>
     <row r="105" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A105" s="12" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B105" s="13" t="s">
         <v>283</v>
@@ -4475,7 +4539,7 @@
     </row>
     <row r="106" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A106" s="12" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B106" s="13" t="s">
         <v>402</v>
@@ -4489,7 +4553,7 @@
     </row>
     <row r="107" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A107" s="12" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B107" s="15" t="s">
         <v>307</v>
@@ -4503,7 +4567,7 @@
     </row>
     <row r="108" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A108" s="12" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B108" s="13" t="s">
         <v>172</v>
@@ -4517,7 +4581,7 @@
     </row>
     <row r="109" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A109" s="12" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B109" s="13" t="s">
         <v>104</v>
@@ -4531,7 +4595,7 @@
     </row>
     <row r="110" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A110" s="12" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B110" s="13" t="s">
         <v>72</v>
@@ -4545,7 +4609,7 @@
     </row>
     <row r="111" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A111" s="12" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B111" s="13" t="s">
         <v>347</v>
@@ -4559,7 +4623,7 @@
     </row>
     <row r="112" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A112" s="12" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B112" s="13" t="s">
         <v>433</v>
@@ -4573,7 +4637,7 @@
     </row>
     <row r="113" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A113" s="12" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B113" s="13" t="s">
         <v>131</v>
@@ -4587,7 +4651,7 @@
     </row>
     <row r="114" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A114" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B114" s="13" t="s">
         <v>74</v>
@@ -4601,7 +4665,7 @@
     </row>
     <row r="115" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A115" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B115" s="13" t="s">
         <v>229</v>
@@ -4615,7 +4679,7 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B116" s="13" t="s">
         <v>216</v>
@@ -4629,7 +4693,7 @@
     </row>
     <row r="117" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A117" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B117" s="15" t="s">
         <v>416</v>
@@ -4643,13 +4707,13 @@
     </row>
     <row r="118" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A118" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B118" s="15" t="s">
         <v>236</v>
       </c>
       <c r="C118" s="14" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D118" s="14" t="b">
         <v>0</v>
@@ -4657,13 +4721,13 @@
     </row>
     <row r="119" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A119" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B119" s="15" t="s">
         <v>170</v>
       </c>
       <c r="C119" s="14" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D119" s="14" t="b">
         <v>0</v>
@@ -4671,13 +4735,13 @@
     </row>
     <row r="120" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A120" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B120" s="15" t="s">
         <v>35</v>
       </c>
       <c r="C120" s="14" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D120" s="14" t="b">
         <v>0</v>
@@ -4685,7 +4749,7 @@
     </row>
     <row r="121" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A121" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B121" s="15" t="s">
         <v>446</v>
@@ -4699,7 +4763,7 @@
     </row>
     <row r="122" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A122" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B122" s="13" t="s">
         <v>373</v>
@@ -4713,7 +4777,7 @@
     </row>
     <row r="123" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A123" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B123" s="13" t="s">
         <v>365</v>
@@ -4727,7 +4791,7 @@
     </row>
     <row r="124" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A124" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B124" s="13" t="s">
         <v>49</v>
@@ -4741,7 +4805,7 @@
     </row>
     <row r="125" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A125" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B125" s="13" t="s">
         <v>293</v>
@@ -4755,7 +4819,7 @@
     </row>
     <row r="126" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A126" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B126" s="13" t="s">
         <v>191</v>
@@ -4769,7 +4833,7 @@
     </row>
     <row r="127" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A127" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B127" s="13" t="s">
         <v>139</v>
@@ -4859,7 +4923,7 @@
         <v>10.06</v>
       </c>
       <c r="C133" s="14" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D133" s="14" t="b">
         <v>0</v>
@@ -4912,7 +4976,7 @@
         <v>25</v>
       </c>
       <c r="B137" s="15" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C137" s="14" t="s">
         <v>201</v>
@@ -5097,7 +5161,7 @@
         <v>163</v>
       </c>
       <c r="C150" s="14" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D150" s="14" t="b">
         <v>0</v>
@@ -5125,7 +5189,7 @@
         <v>110</v>
       </c>
       <c r="C152" s="14" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D152" s="14" t="b">
         <v>0</v>
@@ -5181,7 +5245,7 @@
         <v>222</v>
       </c>
       <c r="C156" s="14" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D156" s="14" t="b">
         <v>0</v>
@@ -5237,7 +5301,7 @@
         <v>12.04</v>
       </c>
       <c r="C160" s="14" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D160" s="14" t="b">
         <v>0</v>
@@ -5318,7 +5382,7 @@
         <v>40</v>
       </c>
       <c r="B166" s="15" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C166" s="14" t="s">
         <v>41</v>
@@ -5363,7 +5427,7 @@
         <v>60</v>
       </c>
       <c r="C169" s="14" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D169" s="14" t="b">
         <v>0</v>
@@ -5710,7 +5774,7 @@
         <v>11</v>
       </c>
       <c r="B194" s="15" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C194" s="14" t="s">
         <v>335</v>
@@ -5920,7 +5984,7 @@
         <v>44</v>
       </c>
       <c r="B209" s="15" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C209" s="14" t="s">
         <v>193</v>
@@ -6007,7 +6071,7 @@
         <v>17.05</v>
       </c>
       <c r="C215" s="14" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D215" s="14" t="b">
         <v>0</v>
@@ -6021,7 +6085,7 @@
         <v>17.059999999999999</v>
       </c>
       <c r="C216" s="14" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D216" s="14" t="b">
         <v>0</v>
@@ -6410,7 +6474,7 @@
         <v>7</v>
       </c>
       <c r="B244" s="15" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C244" s="14" t="s">
         <v>280</v>
@@ -6606,18 +6670,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>218</v>
@@ -6631,7 +6695,7 @@
     </row>
     <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>332</v>
@@ -6645,7 +6709,7 @@
     </row>
     <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>42</v>
@@ -6659,7 +6723,7 @@
     </row>
     <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>84</v>
@@ -6673,7 +6737,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>120</v>
@@ -6687,7 +6751,7 @@
     </row>
     <row r="7" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>82</v>
@@ -6701,7 +6765,7 @@
     </row>
     <row r="8" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>174</v>
@@ -6715,7 +6779,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>204</v>
@@ -6729,7 +6793,7 @@
     </row>
     <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>220</v>
@@ -6743,7 +6807,7 @@
     </row>
     <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>359</v>
@@ -6757,7 +6821,7 @@
     </row>
     <row r="12" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>382</v>
@@ -6771,7 +6835,7 @@
     </row>
     <row r="13" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>440</v>
@@ -6785,7 +6849,7 @@
     </row>
     <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>273</v>
@@ -6799,7 +6863,7 @@
     </row>
     <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>255</v>
@@ -6813,7 +6877,7 @@
     </row>
     <row r="16" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>394</v>
@@ -6827,13 +6891,13 @@
     </row>
     <row r="17" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>385</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D17" s="1" t="b">
         <v>1</v>
@@ -6841,7 +6905,7 @@
     </row>
     <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>198</v>
@@ -6855,7 +6919,7 @@
     </row>
     <row r="19" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>275</v>
@@ -6869,7 +6933,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>53</v>
@@ -6883,7 +6947,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>271</v>
@@ -6897,7 +6961,7 @@
     </row>
     <row r="22" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>186</v>
@@ -6911,7 +6975,7 @@
     </row>
     <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>194</v>
@@ -6925,13 +6989,13 @@
     </row>
     <row r="24" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>245</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D24" s="1" t="b">
         <v>1</v>
@@ -6939,7 +7003,7 @@
     </row>
     <row r="25" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>369</v>
@@ -6953,7 +7017,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>321</v>
@@ -6967,7 +7031,7 @@
     </row>
     <row r="27" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>338</v>
@@ -6981,7 +7045,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B28" s="2">
         <v>3.03</v>
@@ -6995,7 +7059,7 @@
     </row>
     <row r="29" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>259</v>
@@ -7009,7 +7073,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>161</v>
@@ -7023,10 +7087,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>38</v>
@@ -7037,7 +7101,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>78</v>
@@ -7051,7 +7115,7 @@
     </row>
     <row r="33" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>2</v>
@@ -7065,7 +7129,7 @@
     </row>
     <row r="34" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>336</v>
@@ -7079,10 +7143,10 @@
     </row>
     <row r="35" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>79</v>
@@ -7093,10 +7157,10 @@
     </row>
     <row r="36" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>3</v>
@@ -7107,10 +7171,10 @@
     </row>
     <row r="37" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>337</v>
@@ -7121,10 +7185,10 @@
     </row>
     <row r="38" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>268</v>
@@ -7135,10 +7199,10 @@
     </row>
     <row r="39" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>69</v>
@@ -7149,7 +7213,7 @@
     </row>
     <row r="40" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>231</v>
@@ -7163,7 +7227,7 @@
     </row>
     <row r="41" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>144</v>
@@ -7177,7 +7241,7 @@
     </row>
     <row r="42" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>212</v>
@@ -7191,7 +7255,7 @@
     </row>
     <row r="43" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>342</v>
@@ -7205,7 +7269,7 @@
     </row>
     <row r="44" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>261</v>
@@ -7219,7 +7283,7 @@
     </row>
     <row r="45" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>305</v>
@@ -7233,7 +7297,7 @@
     </row>
     <row r="46" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>17</v>
@@ -7247,7 +7311,7 @@
     </row>
     <row r="47" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>448</v>
@@ -7261,7 +7325,7 @@
     </row>
     <row r="48" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>313</v>
@@ -7275,7 +7339,7 @@
     </row>
     <row r="49" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>265</v>
@@ -7289,7 +7353,7 @@
     </row>
     <row r="50" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>400</v>
@@ -7303,7 +7367,7 @@
     </row>
     <row r="51" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>288</v>
@@ -7317,7 +7381,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>422</v>
@@ -7331,7 +7395,7 @@
     </row>
     <row r="53" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>112</v>
@@ -7345,7 +7409,7 @@
     </row>
     <row r="54" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>263</v>
@@ -7359,13 +7423,13 @@
     </row>
     <row r="55" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D55" s="1" t="b">
         <v>1</v>
@@ -7373,7 +7437,7 @@
     </row>
     <row r="56" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>114</v>
@@ -7387,7 +7451,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>157</v>
@@ -7401,7 +7465,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>309</v>
@@ -7415,7 +7479,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>210</v>
@@ -7429,7 +7493,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>99</v>
@@ -7443,7 +7507,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>55</v>
@@ -7457,7 +7521,7 @@
     </row>
     <row r="62" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>328</v>
@@ -7471,7 +7535,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>250</v>
@@ -7485,7 +7549,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>281</v>
@@ -7499,7 +7563,7 @@
     </row>
     <row r="65" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>363</v>
@@ -7513,7 +7577,7 @@
     </row>
     <row r="66" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>442</v>
@@ -7527,7 +7591,7 @@
     </row>
     <row r="67" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>451</v>
@@ -7541,7 +7605,7 @@
     </row>
     <row r="68" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>106</v>
@@ -7555,7 +7619,7 @@
     </row>
     <row r="69" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>296</v>
@@ -7569,7 +7633,7 @@
     </row>
     <row r="70" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>404</v>
@@ -7583,7 +7647,7 @@
     </row>
     <row r="71" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>66</v>
@@ -7597,7 +7661,7 @@
     </row>
     <row r="72" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>298</v>
@@ -7611,7 +7675,7 @@
     </row>
     <row r="73" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>409</v>
@@ -7625,7 +7689,7 @@
     </row>
     <row r="74" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>177</v>
@@ -7639,7 +7703,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>122</v>
@@ -7653,7 +7717,7 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>87</v>
@@ -7667,7 +7731,7 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>51</v>
@@ -7681,7 +7745,7 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>240</v>
@@ -7695,7 +7759,7 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>453</v>
@@ -7709,7 +7773,7 @@
     </row>
     <row r="80" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>184</v>
@@ -7723,7 +7787,7 @@
     </row>
     <row r="81" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>326</v>
@@ -7737,7 +7801,7 @@
     </row>
     <row r="82" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>407</v>
@@ -7751,7 +7815,7 @@
     </row>
     <row r="83" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>458</v>
@@ -7765,7 +7829,7 @@
     </row>
     <row r="84" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>315</v>
@@ -7779,7 +7843,7 @@
     </row>
     <row r="85" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>166</v>
@@ -7793,7 +7857,7 @@
     </row>
     <row r="86" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>76</v>
@@ -7807,7 +7871,7 @@
     </row>
     <row r="87" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>323</v>
@@ -7821,13 +7885,13 @@
     </row>
     <row r="88" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>146</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D88" s="1" t="b">
         <v>0</v>
@@ -7835,7 +7899,7 @@
     </row>
     <row r="89" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>269</v>
@@ -7849,7 +7913,7 @@
     </row>
     <row r="90" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>413</v>
@@ -7863,7 +7927,7 @@
     </row>
     <row r="91" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>444</v>
@@ -7877,7 +7941,7 @@
     </row>
     <row r="92" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>429</v>
@@ -7891,7 +7955,7 @@
     </row>
     <row r="93" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>357</v>
@@ -7905,7 +7969,7 @@
     </row>
     <row r="94" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>340</v>
@@ -7919,7 +7983,7 @@
     </row>
     <row r="95" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>376</v>
@@ -7933,7 +7997,7 @@
     </row>
     <row r="96" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>62</v>
@@ -7947,7 +8011,7 @@
     </row>
     <row r="97" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>283</v>
@@ -7961,7 +8025,7 @@
     </row>
     <row r="98" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>402</v>
@@ -7975,7 +8039,7 @@
     </row>
     <row r="99" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>307</v>
@@ -7989,7 +8053,7 @@
     </row>
     <row r="100" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>172</v>
@@ -8003,7 +8067,7 @@
     </row>
     <row r="101" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>104</v>
@@ -8017,7 +8081,7 @@
     </row>
     <row r="102" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>72</v>
@@ -8031,7 +8095,7 @@
     </row>
     <row r="103" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>347</v>
@@ -8045,7 +8109,7 @@
     </row>
     <row r="104" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>433</v>
@@ -8059,7 +8123,7 @@
     </row>
     <row r="105" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>131</v>
@@ -8073,7 +8137,7 @@
     </row>
     <row r="106" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>74</v>
@@ -8087,7 +8151,7 @@
     </row>
     <row r="107" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>229</v>
@@ -8101,7 +8165,7 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>216</v>
@@ -8115,7 +8179,7 @@
     </row>
     <row r="109" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>416</v>
@@ -8129,7 +8193,7 @@
     </row>
     <row r="110" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B110" s="2" t="s">
         <v>236</v>
@@ -8143,7 +8207,7 @@
     </row>
     <row r="111" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>170</v>
@@ -8157,7 +8221,7 @@
     </row>
     <row r="112" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B112" s="2" t="s">
         <v>35</v>
@@ -8171,7 +8235,7 @@
     </row>
     <row r="113" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>446</v>
@@ -8185,7 +8249,7 @@
     </row>
     <row r="114" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>373</v>
@@ -8199,7 +8263,7 @@
     </row>
     <row r="115" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>365</v>
@@ -8213,7 +8277,7 @@
     </row>
     <row r="116" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B116" s="3" t="s">
         <v>49</v>
@@ -8227,7 +8291,7 @@
     </row>
     <row r="117" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B117" s="3" t="s">
         <v>293</v>
@@ -8241,7 +8305,7 @@
     </row>
     <row r="118" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>191</v>
@@ -8255,7 +8319,7 @@
     </row>
     <row r="119" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B119" s="3" t="s">
         <v>139</v>
@@ -8345,7 +8409,7 @@
         <v>10.06</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D125" s="1" t="b">
         <v>0</v>
@@ -8398,7 +8462,7 @@
         <v>25</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>201</v>
@@ -8804,7 +8868,7 @@
         <v>40</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>41</v>
@@ -9196,7 +9260,7 @@
         <v>11</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C186" s="1" t="s">
         <v>335</v>
@@ -9406,7 +9470,7 @@
         <v>44</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>193</v>
@@ -9493,7 +9557,7 @@
         <v>17.05</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D207" s="1" t="b">
         <v>0</v>
@@ -9507,7 +9571,7 @@
         <v>17.059999999999999</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D208" s="1" t="b">
         <v>0</v>
@@ -9868,7 +9932,7 @@
         <v>7</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C234" s="1" t="s">
         <v>280</v>
@@ -10045,8 +10109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30785CFA-1796-403F-A2BA-36336342C256}">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10057,16 +10121,16 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>486</v>
+      </c>
+      <c r="B1" t="s">
         <v>487</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>488</v>
       </c>
-      <c r="C1" t="s">
-        <v>489</v>
-      </c>
       <c r="D1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F1" s="7"/>
       <c r="G1" s="8"/>
@@ -10074,16 +10138,16 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
+        <v>489</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>490</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>491</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>492</v>
-      </c>
       <c r="D2" s="10" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="5"/>
@@ -10091,16 +10155,16 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>493</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>494</v>
-      </c>
       <c r="C3" s="9" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="8"/>
@@ -10108,16 +10172,16 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
+        <v>494</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>495</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>496</v>
-      </c>
       <c r="C4" s="6" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="5"/>
@@ -10125,16 +10189,16 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="L5" s="4"/>
       <c r="M5" s="5"/>
@@ -10142,16 +10206,16 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
+        <v>497</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>498</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="6" t="s">
         <v>499</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>500</v>
-      </c>
       <c r="D6" s="10" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="L6" s="7"/>
       <c r="M6" s="8"/>
@@ -10159,16 +10223,16 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
+        <v>500</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>501</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>502</v>
-      </c>
       <c r="C7" s="9" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>516</v>
+        <v>532</v>
       </c>
       <c r="L7" s="4"/>
       <c r="M7" s="5"/>
@@ -10176,16 +10240,16 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>516</v>
+        <v>532</v>
       </c>
       <c r="L8" s="7"/>
       <c r="M8" s="8"/>
@@ -10193,16 +10257,16 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="L9" s="4"/>
       <c r="M9" s="5"/>
@@ -10210,16 +10274,16 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="L10" s="7"/>
       <c r="M10" s="8"/>

</xml_diff>

<commit_message>
Updated final review to allow for download of the full report.
</commit_message>
<xml_diff>
--- a/files/compliance_standards.xlsx
+++ b/files/compliance_standards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olato\PycharmProjects\site_qa_review\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C159F4F-4D29-480A-BC7D-7FA58D53FD08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EF43E63-555C-4501-9AF7-6A26CF20A0CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2964" yWindow="2964" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TOBOLA Standards" sheetId="3" r:id="rId1"/>
@@ -2201,7 +2201,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2230,7 +2230,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2343,8 +2342,9 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F56633E1-3A94-4ABD-834C-8F3277A204A4}" name="Table13" displayName="Table13" ref="A1:D255" totalsRowShown="0" dataDxfId="7">
   <autoFilter ref="A1:D255" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B255">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D255">
     <sortCondition ref="A2:A255"/>
+    <sortCondition ref="B2:B255"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{B5F57C1F-71D7-4E66-B159-26F7D14FC333}" name="SECTION" dataDxfId="6"/>
@@ -2675,7 +2675,7 @@
   </sheetPr>
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
@@ -3000,7 +3000,7 @@
       <c r="A23" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B23" t="s">
         <v>535</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -3014,7 +3014,7 @@
       <c r="A24" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" t="s">
         <v>536</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -3028,7 +3028,7 @@
       <c r="A25" t="s">
         <v>96</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B25" t="s">
         <v>538</v>
       </c>
       <c r="C25" s="1" t="s">
@@ -3054,8 +3054,8 @@
   </sheetPr>
   <dimension ref="A1:D255"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A243" workbookViewId="0">
+      <selection activeCell="B254" sqref="B254"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3221,15 +3221,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>463</v>
       </c>
-      <c r="B12" s="15" t="s">
-        <v>204</v>
+      <c r="B12" s="13" t="s">
+        <v>220</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>205</v>
+        <v>221</v>
       </c>
       <c r="D12" s="14" t="b">
         <v>1</v>
@@ -3240,24 +3240,24 @@
         <v>463</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>220</v>
+        <v>359</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>221</v>
+        <v>360</v>
       </c>
       <c r="D13" s="14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
         <v>463</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>359</v>
+        <v>382</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>360</v>
+        <v>383</v>
       </c>
       <c r="D14" s="14" t="b">
         <v>0</v>
@@ -3268,80 +3268,80 @@
         <v>463</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>382</v>
+        <v>440</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>383</v>
+        <v>441</v>
       </c>
       <c r="D15" s="14" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
         <v>463</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>440</v>
+        <v>273</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>441</v>
+        <v>274</v>
       </c>
       <c r="D16" s="14" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
         <v>463</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>273</v>
+        <v>394</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>274</v>
+        <v>395</v>
       </c>
       <c r="D17" s="14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
         <v>463</v>
       </c>
-      <c r="B18" s="15" t="s">
-        <v>255</v>
+      <c r="B18" s="13" t="s">
+        <v>385</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>256</v>
+        <v>386</v>
       </c>
       <c r="D18" s="14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
         <v>463</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>394</v>
+        <v>198</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>395</v>
+        <v>199</v>
       </c>
       <c r="D19" s="14" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
         <v>463</v>
       </c>
-      <c r="B20" s="13" t="s">
-        <v>385</v>
+      <c r="B20" s="15" t="s">
+        <v>204</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>386</v>
+        <v>205</v>
       </c>
       <c r="D20" s="14" t="b">
         <v>1</v>
@@ -3351,14 +3351,14 @@
       <c r="A21" s="12" t="s">
         <v>463</v>
       </c>
-      <c r="B21" s="13" t="s">
-        <v>198</v>
+      <c r="B21" s="15" t="s">
+        <v>255</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>199</v>
+        <v>256</v>
       </c>
       <c r="D21" s="14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -3379,25 +3379,25 @@
       <c r="A23" s="12" t="s">
         <v>470</v>
       </c>
-      <c r="B23" s="15" t="s">
-        <v>53</v>
+      <c r="B23" s="13" t="s">
+        <v>420</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>54</v>
+        <v>421</v>
       </c>
       <c r="D23" s="14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
         <v>470</v>
       </c>
-      <c r="B24" s="15" t="s">
-        <v>271</v>
+      <c r="B24" s="13" t="s">
+        <v>47</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>272</v>
+        <v>48</v>
       </c>
       <c r="D24" s="14" t="b">
         <v>1</v>
@@ -3407,39 +3407,39 @@
       <c r="A25" s="12" t="s">
         <v>470</v>
       </c>
-      <c r="B25" s="15" t="s">
-        <v>186</v>
+      <c r="B25" s="13" t="s">
+        <v>78</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>187</v>
+        <v>79</v>
       </c>
       <c r="D25" s="14" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
         <v>470</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>194</v>
+        <v>53</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>195</v>
+        <v>54</v>
       </c>
       <c r="D26" s="14" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">
         <v>470</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>245</v>
+        <v>271</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>518</v>
+        <v>272</v>
       </c>
       <c r="D27" s="14" t="b">
         <v>1</v>
@@ -3450,94 +3450,94 @@
         <v>470</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>369</v>
+        <v>186</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>370</v>
+        <v>187</v>
       </c>
       <c r="D28" s="14" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="12" t="s">
         <v>470</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>321</v>
+        <v>194</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>322</v>
+        <v>195</v>
       </c>
       <c r="D29" s="14" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="12" t="s">
         <v>470</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>338</v>
+        <v>245</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>339</v>
+        <v>518</v>
       </c>
       <c r="D30" s="14" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="12" t="s">
         <v>470</v>
       </c>
-      <c r="B31" s="13" t="s">
-        <v>420</v>
+      <c r="B31" s="15" t="s">
+        <v>369</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>421</v>
+        <v>370</v>
       </c>
       <c r="D31" s="14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="12" t="s">
         <v>470</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>57</v>
+        <v>321</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>58</v>
+        <v>322</v>
       </c>
       <c r="D32" s="14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A33" s="12" t="s">
         <v>470</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>70</v>
+        <v>338</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>71</v>
+        <v>339</v>
       </c>
       <c r="D33" s="14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="12" t="s">
         <v>470</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="D34" s="14" t="b">
         <v>0</v>
@@ -3547,53 +3547,53 @@
       <c r="A35" s="12" t="s">
         <v>470</v>
       </c>
-      <c r="B35" s="13" t="s">
-        <v>47</v>
+      <c r="B35" s="15" t="s">
+        <v>70</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="D35" s="14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="12" t="s">
         <v>470</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>259</v>
+        <v>37</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>260</v>
+        <v>38</v>
       </c>
       <c r="D36" s="14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="12" t="s">
         <v>470</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>161</v>
+        <v>259</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>162</v>
+        <v>260</v>
       </c>
       <c r="D37" s="14" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A38" s="12" t="s">
         <v>470</v>
       </c>
-      <c r="B38" s="13" t="s">
-        <v>78</v>
+      <c r="B38" s="15" t="s">
+        <v>161</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>79</v>
+        <v>162</v>
       </c>
       <c r="D38" s="14" t="b">
         <v>1</v>
@@ -3753,29 +3753,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A50" s="12" t="s">
         <v>469</v>
       </c>
-      <c r="B50" s="15" t="s">
-        <v>448</v>
+      <c r="B50" s="13" t="s">
+        <v>313</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>449</v>
+        <v>314</v>
       </c>
       <c r="D50" s="14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A51" s="12" t="s">
         <v>469</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>313</v>
+        <v>265</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>314</v>
+        <v>266</v>
       </c>
       <c r="D51" s="14" t="b">
         <v>1</v>
@@ -3786,13 +3786,13 @@
         <v>469</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D52" s="14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -3800,10 +3800,10 @@
         <v>469</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>400</v>
+        <v>448</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>401</v>
+        <v>449</v>
       </c>
       <c r="D53" s="14" t="b">
         <v>0</v>
@@ -3814,55 +3814,55 @@
         <v>469</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>288</v>
+        <v>400</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>289</v>
+        <v>401</v>
       </c>
       <c r="D54" s="14" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A55" s="12" t="s">
         <v>469</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>422</v>
+        <v>288</v>
       </c>
       <c r="C55" s="14" t="s">
-        <v>423</v>
+        <v>289</v>
       </c>
       <c r="D55" s="14" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="12" t="s">
         <v>469</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>112</v>
+        <v>422</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>113</v>
+        <v>423</v>
       </c>
       <c r="D56" s="14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A57" s="12" t="s">
         <v>469</v>
       </c>
-      <c r="B57" s="13" t="s">
-        <v>263</v>
+      <c r="B57" s="15" t="s">
+        <v>112</v>
       </c>
       <c r="C57" s="14" t="s">
-        <v>264</v>
+        <v>113</v>
       </c>
       <c r="D57" s="14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -3879,29 +3879,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A59" s="12" t="s">
         <v>468</v>
       </c>
-      <c r="B59" s="15" t="s">
-        <v>238</v>
+      <c r="B59" s="13" t="s">
+        <v>114</v>
       </c>
       <c r="C59" s="14" t="s">
-        <v>239</v>
+        <v>115</v>
       </c>
       <c r="D59" s="14" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="12" t="s">
         <v>468</v>
       </c>
-      <c r="B60" s="15" t="s">
-        <v>455</v>
+      <c r="B60" s="13" t="s">
+        <v>363</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>456</v>
+        <v>364</v>
       </c>
       <c r="D60" s="14" t="b">
         <v>1</v>
@@ -3911,11 +3911,11 @@
       <c r="A61" s="12" t="s">
         <v>468</v>
       </c>
-      <c r="B61" s="15" t="s">
-        <v>349</v>
+      <c r="B61" s="13" t="s">
+        <v>442</v>
       </c>
       <c r="C61" s="14" t="s">
-        <v>350</v>
+        <v>443</v>
       </c>
       <c r="D61" s="14" t="b">
         <v>1</v>
@@ -3925,11 +3925,11 @@
       <c r="A62" s="12" t="s">
         <v>468</v>
       </c>
-      <c r="B62" s="15" t="s">
-        <v>437</v>
+      <c r="B62" s="13" t="s">
+        <v>298</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>438</v>
+        <v>299</v>
       </c>
       <c r="D62" s="14" t="b">
         <v>1</v>
@@ -3939,28 +3939,28 @@
       <c r="A63" s="12" t="s">
         <v>468</v>
       </c>
-      <c r="B63" s="15" t="s">
-        <v>125</v>
+      <c r="B63" s="13" t="s">
+        <v>409</v>
       </c>
       <c r="C63" s="14" t="s">
-        <v>126</v>
+        <v>410</v>
       </c>
       <c r="D63" s="14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A64" s="12" t="s">
         <v>468</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>114</v>
+        <v>177</v>
       </c>
       <c r="C64" s="14" t="s">
-        <v>115</v>
+        <v>178</v>
       </c>
       <c r="D64" s="14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -3968,10 +3968,10 @@
         <v>468</v>
       </c>
       <c r="B65" s="15" t="s">
-        <v>157</v>
+        <v>238</v>
       </c>
       <c r="C65" s="14" t="s">
-        <v>158</v>
+        <v>239</v>
       </c>
       <c r="D65" s="14" t="b">
         <v>1</v>
@@ -3982,10 +3982,10 @@
         <v>468</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>309</v>
+        <v>455</v>
       </c>
       <c r="C66" s="14" t="s">
-        <v>310</v>
+        <v>456</v>
       </c>
       <c r="D66" s="14" t="b">
         <v>1</v>
@@ -3996,24 +3996,24 @@
         <v>468</v>
       </c>
       <c r="B67" s="15" t="s">
-        <v>210</v>
+        <v>349</v>
       </c>
       <c r="C67" s="14" t="s">
-        <v>211</v>
+        <v>350</v>
       </c>
       <c r="D67" s="14" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A68" s="12" t="s">
         <v>468</v>
       </c>
       <c r="B68" s="15" t="s">
-        <v>99</v>
+        <v>437</v>
       </c>
       <c r="C68" s="14" t="s">
-        <v>100</v>
+        <v>438</v>
       </c>
       <c r="D68" s="14" t="b">
         <v>1</v>
@@ -4024,24 +4024,24 @@
         <v>468</v>
       </c>
       <c r="B69" s="15" t="s">
-        <v>55</v>
+        <v>125</v>
       </c>
       <c r="C69" s="14" t="s">
-        <v>56</v>
+        <v>126</v>
       </c>
       <c r="D69" s="14" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="12" t="s">
         <v>468</v>
       </c>
       <c r="B70" s="15" t="s">
-        <v>328</v>
+        <v>157</v>
       </c>
       <c r="C70" s="14" t="s">
-        <v>329</v>
+        <v>158</v>
       </c>
       <c r="D70" s="14" t="b">
         <v>1</v>
@@ -4052,10 +4052,10 @@
         <v>468</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>250</v>
+        <v>309</v>
       </c>
       <c r="C71" s="14" t="s">
-        <v>251</v>
+        <v>310</v>
       </c>
       <c r="D71" s="14" t="b">
         <v>1</v>
@@ -4066,24 +4066,24 @@
         <v>468</v>
       </c>
       <c r="B72" s="15" t="s">
-        <v>281</v>
+        <v>210</v>
       </c>
       <c r="C72" s="14" t="s">
-        <v>282</v>
+        <v>211</v>
       </c>
       <c r="D72" s="14" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="12" t="s">
         <v>468</v>
       </c>
-      <c r="B73" s="13" t="s">
-        <v>363</v>
+      <c r="B73" s="15" t="s">
+        <v>99</v>
       </c>
       <c r="C73" s="14" t="s">
-        <v>364</v>
+        <v>100</v>
       </c>
       <c r="D73" s="14" t="b">
         <v>1</v>
@@ -4093,126 +4093,126 @@
       <c r="A74" s="12" t="s">
         <v>468</v>
       </c>
-      <c r="B74" s="13" t="s">
-        <v>442</v>
+      <c r="B74" s="15" t="s">
+        <v>55</v>
       </c>
       <c r="C74" s="14" t="s">
-        <v>443</v>
+        <v>56</v>
       </c>
       <c r="D74" s="14" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A75" s="12" t="s">
         <v>468</v>
       </c>
       <c r="B75" s="15" t="s">
-        <v>451</v>
+        <v>328</v>
       </c>
       <c r="C75" s="14" t="s">
-        <v>452</v>
+        <v>329</v>
       </c>
       <c r="D75" s="14" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="12" t="s">
         <v>468</v>
       </c>
       <c r="B76" s="15" t="s">
-        <v>106</v>
+        <v>250</v>
       </c>
       <c r="C76" s="14" t="s">
-        <v>107</v>
+        <v>251</v>
       </c>
       <c r="D76" s="14" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="12" t="s">
         <v>468</v>
       </c>
       <c r="B77" s="15" t="s">
-        <v>296</v>
+        <v>281</v>
       </c>
       <c r="C77" s="14" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
       <c r="D77" s="14" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A78" s="12" t="s">
         <v>468</v>
       </c>
       <c r="B78" s="15" t="s">
-        <v>404</v>
+        <v>451</v>
       </c>
       <c r="C78" s="14" t="s">
-        <v>405</v>
+        <v>452</v>
       </c>
       <c r="D78" s="14" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A79" s="12" t="s">
         <v>468</v>
       </c>
       <c r="B79" s="15" t="s">
-        <v>66</v>
+        <v>106</v>
       </c>
       <c r="C79" s="14" t="s">
-        <v>67</v>
+        <v>107</v>
       </c>
       <c r="D79" s="14" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A80" s="12" t="s">
         <v>468</v>
       </c>
-      <c r="B80" s="13" t="s">
-        <v>298</v>
+      <c r="B80" s="15" t="s">
+        <v>296</v>
       </c>
       <c r="C80" s="14" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D80" s="14" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A81" s="12" t="s">
         <v>468</v>
       </c>
-      <c r="B81" s="13" t="s">
-        <v>409</v>
+      <c r="B81" s="15" t="s">
+        <v>404</v>
       </c>
       <c r="C81" s="14" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="D81" s="14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A82" s="12" t="s">
         <v>468</v>
       </c>
-      <c r="B82" s="13" t="s">
-        <v>177</v>
+      <c r="B82" s="15" t="s">
+        <v>66</v>
       </c>
       <c r="C82" s="14" t="s">
-        <v>178</v>
+        <v>67</v>
       </c>
       <c r="D82" s="14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
@@ -4397,15 +4397,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A96" s="12" t="s">
         <v>466</v>
       </c>
-      <c r="B96" s="15" t="s">
-        <v>146</v>
+      <c r="B96" s="13" t="s">
+        <v>444</v>
       </c>
       <c r="C96" s="14" t="s">
-        <v>522</v>
+        <v>445</v>
       </c>
       <c r="D96" s="14" t="b">
         <v>0</v>
@@ -4415,81 +4415,81 @@
       <c r="A97" s="12" t="s">
         <v>466</v>
       </c>
-      <c r="B97" s="15" t="s">
-        <v>269</v>
+      <c r="B97" s="13" t="s">
+        <v>429</v>
       </c>
       <c r="C97" s="14" t="s">
-        <v>270</v>
+        <v>430</v>
       </c>
       <c r="D97" s="14" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A98" s="12" t="s">
         <v>466</v>
       </c>
-      <c r="B98" s="15" t="s">
-        <v>413</v>
+      <c r="B98" s="13" t="s">
+        <v>357</v>
       </c>
       <c r="C98" s="14" t="s">
-        <v>414</v>
+        <v>358</v>
       </c>
       <c r="D98" s="14" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A99" s="12" t="s">
         <v>466</v>
       </c>
       <c r="B99" s="13" t="s">
-        <v>444</v>
+        <v>340</v>
       </c>
       <c r="C99" s="14" t="s">
-        <v>445</v>
+        <v>341</v>
       </c>
       <c r="D99" s="14" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A100" s="12" t="s">
         <v>466</v>
       </c>
       <c r="B100" s="13" t="s">
-        <v>429</v>
+        <v>376</v>
       </c>
       <c r="C100" s="14" t="s">
-        <v>430</v>
+        <v>377</v>
       </c>
       <c r="D100" s="14" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A101" s="12" t="s">
         <v>466</v>
       </c>
-      <c r="B101" s="13" t="s">
-        <v>357</v>
+      <c r="B101" s="15" t="s">
+        <v>146</v>
       </c>
       <c r="C101" s="14" t="s">
-        <v>358</v>
+        <v>522</v>
       </c>
       <c r="D101" s="14" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A102" s="12" t="s">
         <v>466</v>
       </c>
-      <c r="B102" s="13" t="s">
-        <v>340</v>
+      <c r="B102" s="15" t="s">
+        <v>269</v>
       </c>
       <c r="C102" s="14" t="s">
-        <v>341</v>
+        <v>270</v>
       </c>
       <c r="D102" s="14" t="b">
         <v>0</v>
@@ -4499,11 +4499,11 @@
       <c r="A103" s="12" t="s">
         <v>466</v>
       </c>
-      <c r="B103" s="13" t="s">
-        <v>376</v>
+      <c r="B103" s="15" t="s">
+        <v>413</v>
       </c>
       <c r="C103" s="14" t="s">
-        <v>377</v>
+        <v>414</v>
       </c>
       <c r="D103" s="14" t="b">
         <v>0</v>
@@ -4555,25 +4555,25 @@
       <c r="A107" s="12" t="s">
         <v>465</v>
       </c>
-      <c r="B107" s="15" t="s">
-        <v>307</v>
+      <c r="B107" s="13" t="s">
+        <v>172</v>
       </c>
       <c r="C107" s="14" t="s">
-        <v>308</v>
+        <v>173</v>
       </c>
       <c r="D107" s="14" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A108" s="12" t="s">
         <v>465</v>
       </c>
       <c r="B108" s="13" t="s">
-        <v>172</v>
+        <v>104</v>
       </c>
       <c r="C108" s="14" t="s">
-        <v>173</v>
+        <v>105</v>
       </c>
       <c r="D108" s="14" t="b">
         <v>0</v>
@@ -4584,10 +4584,10 @@
         <v>465</v>
       </c>
       <c r="B109" s="13" t="s">
-        <v>104</v>
+        <v>72</v>
       </c>
       <c r="C109" s="14" t="s">
-        <v>105</v>
+        <v>73</v>
       </c>
       <c r="D109" s="14" t="b">
         <v>0</v>
@@ -4598,55 +4598,55 @@
         <v>465</v>
       </c>
       <c r="B110" s="13" t="s">
-        <v>72</v>
+        <v>347</v>
       </c>
       <c r="C110" s="14" t="s">
-        <v>73</v>
+        <v>348</v>
       </c>
       <c r="D110" s="14" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A111" s="12" t="s">
         <v>465</v>
       </c>
       <c r="B111" s="13" t="s">
-        <v>347</v>
+        <v>433</v>
       </c>
       <c r="C111" s="14" t="s">
-        <v>348</v>
+        <v>434</v>
       </c>
       <c r="D111" s="14" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A112" s="12" t="s">
         <v>465</v>
       </c>
       <c r="B112" s="13" t="s">
-        <v>433</v>
+        <v>131</v>
       </c>
       <c r="C112" s="14" t="s">
-        <v>434</v>
+        <v>132</v>
       </c>
       <c r="D112" s="14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A113" s="12" t="s">
         <v>465</v>
       </c>
-      <c r="B113" s="13" t="s">
-        <v>131</v>
+      <c r="B113" s="15" t="s">
+        <v>307</v>
       </c>
       <c r="C113" s="14" t="s">
-        <v>132</v>
+        <v>308</v>
       </c>
       <c r="D113" s="14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -4691,15 +4691,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A117" s="12" t="s">
         <v>464</v>
       </c>
-      <c r="B117" s="15" t="s">
-        <v>416</v>
+      <c r="B117" s="13" t="s">
+        <v>373</v>
       </c>
       <c r="C117" s="14" t="s">
-        <v>417</v>
+        <v>374</v>
       </c>
       <c r="D117" s="14" t="b">
         <v>0</v>
@@ -4709,11 +4709,11 @@
       <c r="A118" s="12" t="s">
         <v>464</v>
       </c>
-      <c r="B118" s="15" t="s">
-        <v>236</v>
+      <c r="B118" s="13" t="s">
+        <v>365</v>
       </c>
       <c r="C118" s="14" t="s">
-        <v>523</v>
+        <v>366</v>
       </c>
       <c r="D118" s="14" t="b">
         <v>0</v>
@@ -4723,53 +4723,53 @@
       <c r="A119" s="12" t="s">
         <v>464</v>
       </c>
-      <c r="B119" s="15" t="s">
-        <v>170</v>
+      <c r="B119" s="13" t="s">
+        <v>49</v>
       </c>
       <c r="C119" s="14" t="s">
-        <v>524</v>
+        <v>50</v>
       </c>
       <c r="D119" s="14" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A120" s="12" t="s">
         <v>464</v>
       </c>
-      <c r="B120" s="15" t="s">
-        <v>35</v>
+      <c r="B120" s="13" t="s">
+        <v>293</v>
       </c>
       <c r="C120" s="14" t="s">
-        <v>525</v>
+        <v>294</v>
       </c>
       <c r="D120" s="14" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A121" s="12" t="s">
         <v>464</v>
       </c>
-      <c r="B121" s="15" t="s">
-        <v>446</v>
+      <c r="B121" s="13" t="s">
+        <v>191</v>
       </c>
       <c r="C121" s="14" t="s">
-        <v>447</v>
+        <v>192</v>
       </c>
       <c r="D121" s="14" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A122" s="12" t="s">
         <v>464</v>
       </c>
       <c r="B122" s="13" t="s">
-        <v>373</v>
+        <v>139</v>
       </c>
       <c r="C122" s="14" t="s">
-        <v>374</v>
+        <v>140</v>
       </c>
       <c r="D122" s="14" t="b">
         <v>0</v>
@@ -4779,11 +4779,11 @@
       <c r="A123" s="12" t="s">
         <v>464</v>
       </c>
-      <c r="B123" s="13" t="s">
-        <v>365</v>
+      <c r="B123" s="15" t="s">
+        <v>416</v>
       </c>
       <c r="C123" s="14" t="s">
-        <v>366</v>
+        <v>417</v>
       </c>
       <c r="D123" s="14" t="b">
         <v>0</v>
@@ -4793,11 +4793,11 @@
       <c r="A124" s="12" t="s">
         <v>464</v>
       </c>
-      <c r="B124" s="13" t="s">
-        <v>49</v>
+      <c r="B124" s="15" t="s">
+        <v>236</v>
       </c>
       <c r="C124" s="14" t="s">
-        <v>50</v>
+        <v>523</v>
       </c>
       <c r="D124" s="14" t="b">
         <v>0</v>
@@ -4807,11 +4807,11 @@
       <c r="A125" s="12" t="s">
         <v>464</v>
       </c>
-      <c r="B125" s="13" t="s">
-        <v>293</v>
+      <c r="B125" s="15" t="s">
+        <v>170</v>
       </c>
       <c r="C125" s="14" t="s">
-        <v>294</v>
+        <v>524</v>
       </c>
       <c r="D125" s="14" t="b">
         <v>0</v>
@@ -4821,25 +4821,25 @@
       <c r="A126" s="12" t="s">
         <v>464</v>
       </c>
-      <c r="B126" s="13" t="s">
-        <v>191</v>
+      <c r="B126" s="15" t="s">
+        <v>35</v>
       </c>
       <c r="C126" s="14" t="s">
-        <v>192</v>
+        <v>525</v>
       </c>
       <c r="D126" s="14" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A127" s="12" t="s">
         <v>464</v>
       </c>
-      <c r="B127" s="13" t="s">
-        <v>139</v>
+      <c r="B127" s="15" t="s">
+        <v>446</v>
       </c>
       <c r="C127" s="14" t="s">
-        <v>140</v>
+        <v>447</v>
       </c>
       <c r="D127" s="14" t="b">
         <v>0</v>

</xml_diff>